<commit_message>
rozmery po uprave velikosti boxu
</commit_message>
<xml_diff>
--- a/materialy/angry birds.xlsx
+++ b/materialy/angry birds.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>Lenovo</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Asus Zen Pad S 8</t>
+  </si>
+  <si>
+    <t>Nexus 6P</t>
+  </si>
+  <si>
+    <t>DP</t>
   </si>
 </sst>
 </file>
@@ -385,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,20 +680,120 @@
         <v>73</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J8:J9" si="9">E9/C9</f>
+        <f t="shared" ref="J9" si="9">E9/C9</f>
         <v>0.15869140625</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K8:K9" si="10">F9/D9</f>
+        <f t="shared" ref="K9" si="10">F9/D9</f>
         <v>0.60221354166666663</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L8:L9" si="11">G9/E9</f>
+        <f t="shared" ref="L9" si="11">G9/E9</f>
         <v>0.14461538461538462</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M8:M9" si="12">H9/F9</f>
+        <f t="shared" ref="M9" si="12">H9/F9</f>
         <v>7.8918918918918918E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>120</v>
+      </c>
+      <c r="F10">
+        <v>180</v>
+      </c>
+      <c r="J10">
+        <f>E10/F10</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>2560</v>
+      </c>
+      <c r="D11">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>2390</v>
+      </c>
+      <c r="D12">
+        <v>1190</v>
+      </c>
+      <c r="E12">
+        <v>420</v>
+      </c>
+      <c r="F12">
+        <v>630</v>
+      </c>
+      <c r="G12">
+        <v>29</v>
+      </c>
+      <c r="H12">
+        <v>37</v>
+      </c>
+      <c r="J12">
+        <f>E12/F12</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>1920</v>
+      </c>
+      <c r="D13">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1080</v>
+      </c>
+      <c r="D14">
+        <v>1590</v>
+      </c>
+      <c r="E14">
+        <v>310</v>
+      </c>
+      <c r="F14">
+        <v>470</v>
+      </c>
+      <c r="G14">
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+      <c r="J14">
+        <f>E14/F14</f>
+        <v>0.65957446808510634</v>
       </c>
     </row>
   </sheetData>
@@ -696,6 +802,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>